<commit_message>
Corrected some things; removed kcal data; removed historic data for german plots
</commit_message>
<xml_diff>
--- a/output/Anzahl_Reference.xlsx
+++ b/output/Anzahl_Reference.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,10 +478,6 @@
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="n"/>
-      <c r="M1" s="1" t="n"/>
-      <c r="N1" s="1" t="n"/>
-      <c r="O1" s="1" t="n"/>
-      <c r="P1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -491,75 +487,55 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>CEU</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EU</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>EU</t>
+          <t>EU27</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>EU12(EastEU)</t>
+          <t>EU28+CH</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>EU15(WestEU)</t>
+          <t>EU28+CH+NO</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>EU27</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>EU28+CH</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>EU28+CH+NO</t>
+          <t>OrganisationforEconomicCooperationandDevelopment</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>GN</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>IE</t>
-        </is>
-      </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>OrganisationforEconomicCooperationandDevelopment</t>
-        </is>
-      </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>WD</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>WDDLS</t>
         </is>
@@ -578,9 +554,11 @@
           <t>average distance travelled per capita and year</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -588,25 +566,19 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
       <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -616,9 +588,11 @@
           <t>average distance travelled per capita and year | car</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -626,23 +600,17 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -650,9 +618,11 @@
           <t>average distance travelled per capita and year | plane</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -660,25 +630,19 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
-        <v>4</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="n">
-        <v>1</v>
-      </c>
-      <c r="O6" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -686,14 +650,18 @@
           <t>cement production per capita and year</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>1</v>
@@ -703,20 +671,12 @@
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
-        <v>2</v>
-      </c>
-      <c r="O7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -724,37 +684,33 @@
           <t>final energy demand per capita and year</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
       <c r="J8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" t="n">
-        <v>2</v>
-      </c>
-      <c r="O8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
         <v>3</v>
       </c>
-      <c r="P8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -762,12 +718,16 @@
           <t>final energy demand per capita and year | industry</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>1</v>
@@ -777,20 +737,12 @@
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="n">
-        <v>2</v>
-      </c>
-      <c r="O9" t="n">
-        <v>1</v>
-      </c>
-      <c r="P9" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -798,29 +750,25 @@
           <t>food waste per capita and year</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="n">
-        <v>4</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
-        <v>2</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="n">
-        <v>1</v>
-      </c>
-      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -828,117 +776,103 @@
           <t>living space per capita</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
       <c r="G11" t="n">
         <v>1</v>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
-        <v>1</v>
-      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
         <v>1</v>
       </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="n">
-        <v>1</v>
-      </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" t="n">
-        <v>2</v>
-      </c>
-      <c r="P11" t="inlineStr"/>
+      <c r="K11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>meat consumption per capita and day</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1</v>
-      </c>
+          <t>per capita floor area in commercial and public buildings</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="n">
-        <v>1</v>
-      </c>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" t="n">
-        <v>1</v>
-      </c>
-      <c r="P12" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>per capita floor area in commercial and public buildings</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
+          <t>steel production per capita and year</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>3</v>
+      </c>
       <c r="C13" t="n">
         <v>1</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
       <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="n">
-        <v>2</v>
-      </c>
-      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>steel production per capita and year</t>
+          <t>transported goods per capita and year</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
-      </c>
-      <c r="D14" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
@@ -951,58 +885,14 @@
       <c r="J14" t="n">
         <v>1</v>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="n">
-        <v>1</v>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="n">
-        <v>2</v>
-      </c>
-      <c r="O14" t="n">
-        <v>1</v>
-      </c>
-      <c r="P14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>transported goods per capita and year</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="n">
-        <v>1</v>
-      </c>
-      <c r="O15" t="n">
-        <v>2</v>
-      </c>
-      <c r="P15" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected error of hatching. Added data export for barplot
</commit_message>
<xml_diff>
--- a/output/Anzahl_Reference.xlsx
+++ b/output/Anzahl_Reference.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,6 @@
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
-      <c r="L1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -502,40 +501,35 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>EU28+CH</t>
+          <t>EU28+CH+NO</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>EU28+CH+NO</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>OrganisationforEconomicCooperationandDevelopment</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>OrganisationforEconomicCooperationandDevelopment</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>WD</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>WDDLS</t>
         </is>
@@ -564,21 +558,20 @@
         <v>1</v>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
       <c r="G4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
       <c r="J4" t="n">
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -589,7 +582,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -598,19 +591,18 @@
         <v>1</v>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
       <c r="G5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -619,7 +611,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -628,21 +620,20 @@
         <v>1</v>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
       <c r="G6" t="n">
-        <v>4</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
       <c r="J6" t="n">
         <v>1</v>
       </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -651,7 +642,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -659,24 +650,21 @@
       <c r="D7" t="n">
         <v>1</v>
       </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
-      <c r="H7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
       <c r="J7" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -685,16 +673,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>2</v>
       </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" t="n">
         <v>1</v>
       </c>
@@ -702,15 +690,12 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" t="n">
         <v>3</v>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -719,30 +704,27 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>1</v>
       </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
       <c r="G9" t="n">
         <v>1</v>
       </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
       <c r="J9" t="n">
-        <v>2</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -750,25 +732,20 @@
           <t>food waste per capita and year</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>1</v>
       </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -783,24 +760,23 @@
       <c r="D11" t="n">
         <v>1</v>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
       <c r="F11" t="n">
         <v>1</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
       </c>
-      <c r="H11" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
       <c r="J11" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" t="n">
-        <v>2</v>
-      </c>
-      <c r="L11" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -808,9 +784,7 @@
           <t>per capita floor area in commercial and public buildings</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -818,11 +792,10 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
-        <v>2</v>
-      </c>
-      <c r="L12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -831,7 +804,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -839,24 +812,21 @@
       <c r="D13" t="n">
         <v>1</v>
       </c>
-      <c r="E13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
       <c r="G13" t="n">
         <v>1</v>
       </c>
-      <c r="H13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
       <c r="J13" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -865,7 +835,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
@@ -874,25 +844,24 @@
         <v>1</v>
       </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
       <c r="G14" t="n">
         <v>1</v>
       </c>
-      <c r="H14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
       <c r="J14" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" t="n">
-        <v>2</v>
-      </c>
-      <c r="L14" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="K14" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Splitted traffic and non-traffic for barplot. Added color schemes for traffic plots Formatting checked
</commit_message>
<xml_diff>
--- a/output/Anzahl_Reference.xlsx
+++ b/output/Anzahl_Reference.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,11 @@
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -496,40 +501,65 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
+          <t>EU12(EastEU)</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>EU15(WestEU)</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
           <t>EU27</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>EU28</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>EU28+CH+NO</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>FR</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>GN</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>GS</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>IE</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>OrganisationforEconomicCooperationandDevelopment</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>WD</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>WDDLS</t>
         </is>
@@ -554,24 +584,31 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -587,22 +624,35 @@
       <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -616,24 +666,31 @@
       <c r="C6" t="n">
         <v>1</v>
       </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="n">
+        <v>2</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -642,14 +699,12 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>1</v>
@@ -659,12 +714,21 @@
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -676,9 +740,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
-        <v>2</v>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>1</v>
@@ -686,16 +748,25 @@
       <c r="G8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O8" t="n">
         <v>3</v>
       </c>
-      <c r="K8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -707,9 +778,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>1</v>
@@ -719,12 +788,21 @@
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -734,18 +812,23 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>2</v>
-      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -757,81 +840,98 @@
         <v>2</v>
       </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1</v>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>1</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
       <c r="I11" t="n">
         <v>1</v>
       </c>
-      <c r="J11" t="n">
-        <v>2</v>
-      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>2</v>
+      </c>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>per capita floor area in commercial and public buildings</t>
+          <t>meat consumption per capita and day</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>steel production per capita and year</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
+          <t>per capita floor area in commercial and public buildings</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
-        <v>2</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="n">
+        <v>2</v>
+      </c>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>transported goods per capita and year</t>
+          <t>steel production per capita and year</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -840,9 +940,7 @@
       <c r="C14" t="n">
         <v>1</v>
       </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
         <v>1</v>
@@ -854,14 +952,61 @@
       <c r="I14" t="n">
         <v>1</v>
       </c>
-      <c r="J14" t="n">
-        <v>2</v>
-      </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="n">
+        <v>2</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>transported goods per capita and year</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B1:P1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>